<commit_message>
CẬP XONG CROSS, ARRAY, TREATMENT 04.31_10.06
</commit_message>
<xml_diff>
--- a/Xp03-Fabrication & Listing.xlsx
+++ b/Xp03-Fabrication & Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Desktop\thu nghien software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{873FC4D0-28C4-4996-A8FF-A2C48168EE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429B5183-935B-49F1-ABAC-FCBDCF8C86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{8FDBA56C-462C-41E1-BBC9-9F20F3423F7B}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{8FDBA56C-462C-41E1-BBC9-9F20F3423F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Pipe Schedule" sheetId="3" r:id="rId1"/>
@@ -1141,9 +1141,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1379,10 +1376,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1403,10 +1396,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1423,10 +1412,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1553,11 +1538,6 @@
         <name val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
       </font>
     </dxf>
     <dxf>
@@ -1993,6 +1973,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2478,29 +2478,29 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E9F823F9-1E86-48CB-AC15-0B1DEA400BB3}" name="Table2" displayName="Table2" ref="A1:W455" totalsRowCount="1" totalsRowDxfId="112">
   <autoFilter ref="A1:W454" xr:uid="{E9F823F9-1E86-48CB-AC15-0B1DEA400BB3}"/>
   <tableColumns count="23">
-    <tableColumn id="3" xr3:uid="{7BE93B07-3A8D-4BED-9BA0-28E12D30D26F}" name="EE_Cross Passage" totalsRowLabel="Total" totalsRowDxfId="22"/>
-    <tableColumn id="1" xr3:uid="{C161E31C-7076-4341-B499-D7167B5846FE}" name="EE_Location and Lanes" totalsRowDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{E9533709-AEF2-4852-BDB7-245DE4CE2BD1}" name="EE_System Type" totalsRowDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{4C72782C-1613-40F9-8102-035194F99773}" name="EE_Array Number" totalsRowDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{FCDEEFF8-477B-46BD-869A-83971B65E134}" name="EE_Stock Code" totalsRowDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{03431DAD-5635-4B22-AC67-1B57BC2C78A7}" name="EE_Item Description" totalsRowDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{14B02D92-E166-4E66-85C3-6EA8E3805634}" name="Size" totalsRowDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{27E07FD0-7F33-415D-9403-6E310AB7C233}" name="Outside Diameter" dataDxfId="111" totalsRowDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{AB045377-9733-4AE8-8337-840396E40382}" name="Qty" totalsRowFunction="sum" dataDxfId="110" totalsRowDxfId="14"/>
-    <tableColumn id="10" xr3:uid="{068B39DE-386D-4FEB-A53C-B4CD2A827819}" name="Length" dataDxfId="109" totalsRowDxfId="13"/>
-    <tableColumn id="11" xr3:uid="{DB9EE51D-435F-4DC8-9992-D104D839E16C}" name="EE_FAB Pipe" totalsRowDxfId="12"/>
-    <tableColumn id="12" xr3:uid="{4B32BCC0-6A3E-4732-98CD-642D415BDE77}" name="EE_PIPE END-1" totalsRowDxfId="11"/>
-    <tableColumn id="13" xr3:uid="{1BC086BA-0DCD-4938-BC24-0AC7FF5E19CF}" name="EE_PIPE END-2" totalsRowDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{F34DE216-EBE8-4E43-9EF7-0925D99B6809}" name="EE_Run Dim 1" totalsRowDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{D4D8955C-0C13-454B-90AC-C5900827E436}" name="EE_Pap 1" totalsRowDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{F494A82E-7216-4064-B216-D6DC1685A1DF}" name="EE_Run Dim 2" totalsRowDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{ADB4602C-4682-4AC2-BBD0-179D6C099C77}" name="EE_Pap 2" totalsRowDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{DF489165-B65D-4029-AF93-F3288C25ED43}" name="EE_Run Dim 3" totalsRowDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{5EC7BC45-15ED-4547-8C52-033B169A8E0C}" name="EE_Pap 3" totalsRowDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{CD0C63B4-116B-4113-82C6-9CE54D729450}" name="EE_Pipe Treatment" totalsRowDxfId="3"/>
-    <tableColumn id="21" xr3:uid="{215CED18-34F7-4F95-88E1-123503371798}" name="Family" totalsRowDxfId="2"/>
-    <tableColumn id="22" xr3:uid="{F102F050-63CF-4F9C-8432-B6E9BF2E62B4}" name="Type" totalsRowDxfId="1"/>
-    <tableColumn id="23" xr3:uid="{2A0D3495-0144-437B-8CBA-B26F62247857}" name="ID" dataDxfId="108" totalsRowDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{7BE93B07-3A8D-4BED-9BA0-28E12D30D26F}" name="EE_Cross Passage" totalsRowLabel="Total" totalsRowDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{C161E31C-7076-4341-B499-D7167B5846FE}" name="EE_Location and Lanes" totalsRowDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{E9533709-AEF2-4852-BDB7-245DE4CE2BD1}" name="EE_System Type" totalsRowDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{4C72782C-1613-40F9-8102-035194F99773}" name="EE_Array Number" totalsRowDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{FCDEEFF8-477B-46BD-869A-83971B65E134}" name="EE_Stock Code" totalsRowDxfId="41"/>
+    <tableColumn id="6" xr3:uid="{03431DAD-5635-4B22-AC67-1B57BC2C78A7}" name="EE_Item Description" totalsRowDxfId="40"/>
+    <tableColumn id="7" xr3:uid="{14B02D92-E166-4E66-85C3-6EA8E3805634}" name="Size" totalsRowDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{27E07FD0-7F33-415D-9403-6E310AB7C233}" name="Outside Diameter" dataDxfId="111" totalsRowDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{AB045377-9733-4AE8-8337-840396E40382}" name="Qty" totalsRowFunction="sum" dataDxfId="110" totalsRowDxfId="37"/>
+    <tableColumn id="10" xr3:uid="{068B39DE-386D-4FEB-A53C-B4CD2A827819}" name="Length" dataDxfId="109" totalsRowDxfId="36"/>
+    <tableColumn id="11" xr3:uid="{DB9EE51D-435F-4DC8-9992-D104D839E16C}" name="EE_FAB Pipe" totalsRowDxfId="35"/>
+    <tableColumn id="12" xr3:uid="{4B32BCC0-6A3E-4732-98CD-642D415BDE77}" name="EE_PIPE END-1" totalsRowDxfId="34"/>
+    <tableColumn id="13" xr3:uid="{1BC086BA-0DCD-4938-BC24-0AC7FF5E19CF}" name="EE_PIPE END-2" totalsRowDxfId="33"/>
+    <tableColumn id="14" xr3:uid="{F34DE216-EBE8-4E43-9EF7-0925D99B6809}" name="EE_Run Dim 1" totalsRowDxfId="32"/>
+    <tableColumn id="15" xr3:uid="{D4D8955C-0C13-454B-90AC-C5900827E436}" name="EE_Pap 1" totalsRowDxfId="31"/>
+    <tableColumn id="16" xr3:uid="{F494A82E-7216-4064-B216-D6DC1685A1DF}" name="EE_Run Dim 2" totalsRowDxfId="30"/>
+    <tableColumn id="17" xr3:uid="{ADB4602C-4682-4AC2-BBD0-179D6C099C77}" name="EE_Pap 2" totalsRowDxfId="29"/>
+    <tableColumn id="18" xr3:uid="{DF489165-B65D-4029-AF93-F3288C25ED43}" name="EE_Run Dim 3" totalsRowDxfId="28"/>
+    <tableColumn id="19" xr3:uid="{5EC7BC45-15ED-4547-8C52-033B169A8E0C}" name="EE_Pap 3" totalsRowDxfId="27"/>
+    <tableColumn id="20" xr3:uid="{CD0C63B4-116B-4113-82C6-9CE54D729450}" name="EE_Pipe Treatment" totalsRowDxfId="26"/>
+    <tableColumn id="21" xr3:uid="{215CED18-34F7-4F95-88E1-123503371798}" name="Family" totalsRowDxfId="25"/>
+    <tableColumn id="22" xr3:uid="{F102F050-63CF-4F9C-8432-B6E9BF2E62B4}" name="Type" totalsRowDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{2A0D3495-0144-437B-8CBA-B26F62247857}" name="ID" dataDxfId="108" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2542,61 +2542,61 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CE1B34E3-CAD9-4F1E-818D-CDAB205C3051}" name="Table1" displayName="Table1" ref="A1:W518" totalsRowCount="1" totalsRowDxfId="78">
   <autoFilter ref="A1:W517" xr:uid="{CE1B34E3-CAD9-4F1E-818D-CDAB205C3051}"/>
   <tableColumns count="23">
-    <tableColumn id="3" xr3:uid="{7A654B22-8774-4925-8C16-2B1556AFFB7F}" name="EE_Cross Passage" totalsRowLabel="Total" totalsRowDxfId="77"/>
-    <tableColumn id="1" xr3:uid="{9C9D6AA2-051C-430F-BDB6-24FDE207AA20}" name="EE_Location and Lanes" totalsRowDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{74171881-E052-402E-844B-2EDC96AE9018}" name="EE_System Type" totalsRowDxfId="75"/>
-    <tableColumn id="4" xr3:uid="{8C011382-CB13-4A8E-874F-75D509765B0A}" name="EE_Array Number" totalsRowDxfId="74"/>
-    <tableColumn id="5" xr3:uid="{CCE971F0-7CC6-47D3-A559-58537DACAEB9}" name="EE_Stock Code" totalsRowDxfId="73"/>
-    <tableColumn id="6" xr3:uid="{79A1C310-5F92-4986-A323-3D7ABC96900F}" name="EE_Item Description" totalsRowDxfId="72"/>
-    <tableColumn id="7" xr3:uid="{E7418DDE-71E5-42B4-9B9C-0376367302F3}" name="Size" totalsRowDxfId="71"/>
-    <tableColumn id="8" xr3:uid="{6B07EAE2-5E7E-4E3F-8B61-4C282621A947}" name="Outside Diameter" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="9" xr3:uid="{EAFA6AF4-5B0B-44C3-B425-5752B1D35FF8}" name="Qty" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{E93FD4C1-D273-47B1-A83C-06CBEC9AC750}" name="Length" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="11" xr3:uid="{9FEC5CA8-A25E-4490-BD27-D729E9372C50}" name="EE_FAB Pipe" totalsRowDxfId="64"/>
-    <tableColumn id="12" xr3:uid="{5A7ACFD8-C7C6-4BBB-BB8F-466BAB58D9CF}" name="EE_PIPE END-1" totalsRowDxfId="63"/>
-    <tableColumn id="13" xr3:uid="{CA0703FB-D6ED-4D53-92DA-12BFAB200657}" name="EE_PIPE END-2" totalsRowDxfId="62"/>
-    <tableColumn id="14" xr3:uid="{C9715951-249F-401A-8E72-DBBDF55D95C9}" name="EE_Run Dim 1" totalsRowDxfId="61"/>
-    <tableColumn id="15" xr3:uid="{4C0E0BA8-747C-4004-949D-97A713137620}" name="EE_Pap 1" totalsRowDxfId="60"/>
-    <tableColumn id="16" xr3:uid="{9512F8A3-9031-478B-8FE2-6A8D918FE7CF}" name="EE_Run Dim 2" totalsRowDxfId="59"/>
-    <tableColumn id="17" xr3:uid="{F1F6EE04-0A46-499A-851E-94688F44C98D}" name="EE_Pap 2" totalsRowDxfId="58"/>
-    <tableColumn id="18" xr3:uid="{B8BC2317-88CC-43D8-96AC-0FD8FBA4BDEA}" name="EE_Run Dim 3" totalsRowDxfId="57"/>
-    <tableColumn id="19" xr3:uid="{15D3CFDB-9064-4D32-8FCB-E48C236B9216}" name="EE_Pap 3" totalsRowDxfId="56"/>
-    <tableColumn id="20" xr3:uid="{533220B8-ADBE-4D94-8809-B9DB4D59514E}" name="EE_Pipe Treatment" totalsRowDxfId="55"/>
-    <tableColumn id="21" xr3:uid="{0C1FE73C-C87A-486C-B791-BB81594E372F}" name="Family" totalsRowDxfId="54"/>
-    <tableColumn id="22" xr3:uid="{B5D459F5-39F6-4672-ABAA-3CCBB0530311}" name="Type" totalsRowDxfId="53"/>
-    <tableColumn id="23" xr3:uid="{103C5F66-C275-44B6-A167-C35372D6941E}" name="ID" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{7A654B22-8774-4925-8C16-2B1556AFFB7F}" name="EE_Cross Passage" totalsRowLabel="Total" totalsRowDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{9C9D6AA2-051C-430F-BDB6-24FDE207AA20}" name="EE_Location and Lanes" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{74171881-E052-402E-844B-2EDC96AE9018}" name="EE_System Type" totalsRowDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{8C011382-CB13-4A8E-874F-75D509765B0A}" name="EE_Array Number" totalsRowDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{CCE971F0-7CC6-47D3-A559-58537DACAEB9}" name="EE_Stock Code" totalsRowDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{79A1C310-5F92-4986-A323-3D7ABC96900F}" name="EE_Item Description" totalsRowDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{E7418DDE-71E5-42B4-9B9C-0376367302F3}" name="Size" totalsRowDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{6B07EAE2-5E7E-4E3F-8B61-4C282621A947}" name="Outside Diameter" dataDxfId="77" totalsRowDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{EAFA6AF4-5B0B-44C3-B425-5752B1D35FF8}" name="Qty" totalsRowFunction="sum" dataDxfId="76" totalsRowDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{E93FD4C1-D273-47B1-A83C-06CBEC9AC750}" name="Length" dataDxfId="75" totalsRowDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{9FEC5CA8-A25E-4490-BD27-D729E9372C50}" name="EE_FAB Pipe" totalsRowDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{5A7ACFD8-C7C6-4BBB-BB8F-466BAB58D9CF}" name="EE_PIPE END-1" totalsRowDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{CA0703FB-D6ED-4D53-92DA-12BFAB200657}" name="EE_PIPE END-2" totalsRowDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{C9715951-249F-401A-8E72-DBBDF55D95C9}" name="EE_Run Dim 1" totalsRowDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{4C0E0BA8-747C-4004-949D-97A713137620}" name="EE_Pap 1" totalsRowDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{9512F8A3-9031-478B-8FE2-6A8D918FE7CF}" name="EE_Run Dim 2" totalsRowDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{F1F6EE04-0A46-499A-851E-94688F44C98D}" name="EE_Pap 2" totalsRowDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{B8BC2317-88CC-43D8-96AC-0FD8FBA4BDEA}" name="EE_Run Dim 3" totalsRowDxfId="5"/>
+    <tableColumn id="19" xr3:uid="{15D3CFDB-9064-4D32-8FCB-E48C236B9216}" name="EE_Pap 3" totalsRowDxfId="4"/>
+    <tableColumn id="20" xr3:uid="{533220B8-ADBE-4D94-8809-B9DB4D59514E}" name="EE_Pipe Treatment" totalsRowDxfId="3"/>
+    <tableColumn id="21" xr3:uid="{0C1FE73C-C87A-486C-B791-BB81594E372F}" name="Family" totalsRowDxfId="2"/>
+    <tableColumn id="22" xr3:uid="{B5D459F5-39F6-4672-ABAA-3CCBB0530311}" name="Type" totalsRowDxfId="1"/>
+    <tableColumn id="23" xr3:uid="{103C5F66-C275-44B6-A167-C35372D6941E}" name="ID" dataDxfId="74" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{043FF555-5FEC-4A86-BEE6-E93E94FFE95A}" name="Table4" displayName="Table4" ref="A1:W170" totalsRowCount="1" totalsRowDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{043FF555-5FEC-4A86-BEE6-E93E94FFE95A}" name="Table4" displayName="Table4" ref="A1:W170" totalsRowCount="1" totalsRowDxfId="73">
   <autoFilter ref="A1:W169" xr:uid="{043FF555-5FEC-4A86-BEE6-E93E94FFE95A}"/>
   <tableColumns count="23">
-    <tableColumn id="3" xr3:uid="{D1107597-94D4-4E28-B62A-3E6D4D73EB98}" name="EE_Cross Passage" totalsRowLabel="Total" totalsRowDxfId="49"/>
-    <tableColumn id="1" xr3:uid="{9EC8100F-03D4-493F-8DAF-8E2C79473F40}" name="EE_Location and Lanes" totalsRowDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{B81C59DF-796C-40BE-A9C0-F7B7F8F971B2}" name="EE_System Type" totalsRowDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{7AABF85F-E40F-433F-92DF-9A04DCFA8378}" name="EE_Array Number" totalsRowDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{21F55447-2DEC-47FE-8993-0848A32651AE}" name="EE_Stock Code" totalsRowDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{215B6367-2EAC-48B8-9114-0C333F6EACBD}" name="EE_Item Description" totalsRowDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{81D8B348-0339-4DEE-912B-AD0C6D0C3F41}" name="Size" totalsRowDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{2D861A8E-3E3E-4966-B222-6E3422F31DC0}" name="Outside Diameter" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="9" xr3:uid="{6F539BE7-9C6E-48A0-8D0A-A5C151E8C2E2}" name="Qty" totalsRowFunction="sum" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{178DC0E4-61D4-4553-BFE1-07AE23A6BB5E}" name="Length" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{C11F5783-61A5-41A8-BF4C-5D51FBC1DF85}" name="EE_FAB Pipe" totalsRowDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{E4623EEA-B67C-4F14-9EAF-7C93B3289BF9}" name="EE_PIPE END-1" totalsRowDxfId="35"/>
-    <tableColumn id="13" xr3:uid="{B7CEBE0C-02CD-47D0-83F7-3B4B164BC286}" name="EE_PIPE END-2" totalsRowDxfId="34"/>
-    <tableColumn id="14" xr3:uid="{6D4A35DB-9CA1-4629-9075-CF53F4F50C0F}" name="EE_Run Dim 1" totalsRowDxfId="33"/>
-    <tableColumn id="15" xr3:uid="{02C6726F-5A90-4749-ACCC-A0E108426CFE}" name="EE_Pap 1" totalsRowDxfId="32"/>
-    <tableColumn id="16" xr3:uid="{3D284A36-93BA-4F05-B5FB-25E3AB86AE27}" name="EE_Run Dim 2" totalsRowDxfId="31"/>
-    <tableColumn id="17" xr3:uid="{38E20EC6-D1D8-474C-A5D7-FE855968F8FE}" name="EE_Pap 2" totalsRowDxfId="30"/>
-    <tableColumn id="18" xr3:uid="{DDF7BDD5-B054-451D-9B45-DDAA7E5F4776}" name="EE_Run Dim 3" totalsRowDxfId="29"/>
-    <tableColumn id="19" xr3:uid="{E557B280-6897-402D-B962-50AEB731A81A}" name="EE_Pap 3" totalsRowDxfId="28"/>
-    <tableColumn id="20" xr3:uid="{82500CEE-83BA-4267-A222-7D53AFD601D5}" name="EE_Pipe Treatment" totalsRowDxfId="27"/>
-    <tableColumn id="21" xr3:uid="{0A4C255F-1B78-42C4-B713-F08617D295D1}" name="Family" totalsRowDxfId="26"/>
-    <tableColumn id="22" xr3:uid="{163B8372-4555-4625-9275-C4A9FBFF9C3A}" name="Type" totalsRowDxfId="25"/>
-    <tableColumn id="23" xr3:uid="{DFEA8C9A-5981-40FD-B643-9EE18FDE239F}" name="ID" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{D1107597-94D4-4E28-B62A-3E6D4D73EB98}" name="EE_Cross Passage" totalsRowLabel="Total" totalsRowDxfId="72"/>
+    <tableColumn id="1" xr3:uid="{9EC8100F-03D4-493F-8DAF-8E2C79473F40}" name="EE_Location and Lanes" totalsRowDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{B81C59DF-796C-40BE-A9C0-F7B7F8F971B2}" name="EE_System Type" totalsRowDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{7AABF85F-E40F-433F-92DF-9A04DCFA8378}" name="EE_Array Number" totalsRowDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{21F55447-2DEC-47FE-8993-0848A32651AE}" name="EE_Stock Code" totalsRowDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{215B6367-2EAC-48B8-9114-0C333F6EACBD}" name="EE_Item Description" totalsRowDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{81D8B348-0339-4DEE-912B-AD0C6D0C3F41}" name="Size" totalsRowDxfId="66"/>
+    <tableColumn id="8" xr3:uid="{2D861A8E-3E3E-4966-B222-6E3422F31DC0}" name="Outside Diameter" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="9" xr3:uid="{6F539BE7-9C6E-48A0-8D0A-A5C151E8C2E2}" name="Qty" totalsRowFunction="sum" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{178DC0E4-61D4-4553-BFE1-07AE23A6BB5E}" name="Length" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="11" xr3:uid="{C11F5783-61A5-41A8-BF4C-5D51FBC1DF85}" name="EE_FAB Pipe" totalsRowDxfId="59"/>
+    <tableColumn id="12" xr3:uid="{E4623EEA-B67C-4F14-9EAF-7C93B3289BF9}" name="EE_PIPE END-1" totalsRowDxfId="58"/>
+    <tableColumn id="13" xr3:uid="{B7CEBE0C-02CD-47D0-83F7-3B4B164BC286}" name="EE_PIPE END-2" totalsRowDxfId="57"/>
+    <tableColumn id="14" xr3:uid="{6D4A35DB-9CA1-4629-9075-CF53F4F50C0F}" name="EE_Run Dim 1" totalsRowDxfId="56"/>
+    <tableColumn id="15" xr3:uid="{02C6726F-5A90-4749-ACCC-A0E108426CFE}" name="EE_Pap 1" totalsRowDxfId="55"/>
+    <tableColumn id="16" xr3:uid="{3D284A36-93BA-4F05-B5FB-25E3AB86AE27}" name="EE_Run Dim 2" totalsRowDxfId="54"/>
+    <tableColumn id="17" xr3:uid="{38E20EC6-D1D8-474C-A5D7-FE855968F8FE}" name="EE_Pap 2" totalsRowDxfId="53"/>
+    <tableColumn id="18" xr3:uid="{DDF7BDD5-B054-451D-9B45-DDAA7E5F4776}" name="EE_Run Dim 3" totalsRowDxfId="52"/>
+    <tableColumn id="19" xr3:uid="{E557B280-6897-402D-B962-50AEB731A81A}" name="EE_Pap 3" totalsRowDxfId="51"/>
+    <tableColumn id="20" xr3:uid="{82500CEE-83BA-4267-A222-7D53AFD601D5}" name="EE_Pipe Treatment" totalsRowDxfId="50"/>
+    <tableColumn id="21" xr3:uid="{0A4C255F-1B78-42C4-B713-F08617D295D1}" name="Family" totalsRowDxfId="49"/>
+    <tableColumn id="22" xr3:uid="{163B8372-4555-4625-9275-C4A9FBFF9C3A}" name="Type" totalsRowDxfId="48"/>
+    <tableColumn id="23" xr3:uid="{DFEA8C9A-5981-40FD-B643-9EE18FDE239F}" name="ID" dataDxfId="47" totalsRowDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2921,8 +2921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A8B5516-023D-46F5-A4D7-01C8C25EC2E6}">
   <dimension ref="A1:X455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U41" sqref="U41"/>
+    <sheetView topLeftCell="G210" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T278" sqref="T278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3302,7 +3302,7 @@
         <v>82</v>
       </c>
       <c r="T7" t="s">
-        <v>29</v>
+        <v>195</v>
       </c>
       <c r="V7" t="s">
         <v>83</v>
@@ -4934,7 +4934,7 @@
         <v>82</v>
       </c>
       <c r="T41" t="s">
-        <v>195</v>
+        <v>29</v>
       </c>
       <c r="V41" t="s">
         <v>93</v>
@@ -14840,7 +14840,7 @@
         <v>82</v>
       </c>
       <c r="T228" t="s">
-        <v>29</v>
+        <v>195</v>
       </c>
       <c r="V228" t="s">
         <v>93</v>
@@ -17432,7 +17432,7 @@
         <v>108</v>
       </c>
       <c r="T277" t="s">
-        <v>29</v>
+        <v>195</v>
       </c>
       <c r="V277" t="s">
         <v>96</v>
@@ -26156,7 +26156,7 @@
   <dimension ref="A1:X880"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -62635,8 +62635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C34D35-87DC-4E57-AA60-56AEEF5BA330}">
   <dimension ref="A1:X518"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I68" sqref="I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -63927,7 +63927,7 @@
       <c r="J31" s="1"/>
       <c r="K31"/>
       <c r="T31" t="s">
-        <v>195</v>
+        <v>29</v>
       </c>
       <c r="U31" t="s">
         <v>38</v>
@@ -65916,7 +65916,7 @@
       <c r="J82" s="1"/>
       <c r="K82"/>
       <c r="T82" t="s">
-        <v>29</v>
+        <v>195</v>
       </c>
       <c r="U82" t="s">
         <v>39</v>

</xml_diff>